<commit_message>
improved README, added some words to .xslx file
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="words" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
   <si>
     <t>en</t>
   </si>
@@ -260,6 +260,117 @@
     <t>Andiamo</t>
   </si>
   <si>
+    <t>forest</t>
+  </si>
+  <si>
+    <t>bosco</t>
+  </si>
+  <si>
+    <t>see</t>
+  </si>
+  <si>
+    <t>vedere</t>
+  </si>
+  <si>
+    <t>come</t>
+  </si>
+  <si>
+    <t>venire</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>ora</t>
+  </si>
+  <si>
+    <t>tomorrow</t>
+  </si>
+  <si>
+    <t>domani</t>
+  </si>
+  <si>
+    <t>today</t>
+  </si>
+  <si>
+    <t>oggi</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>settimana</t>
+  </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>facile</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>good night</t>
+  </si>
+  <si>
+    <t>Buonanotte</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>caffè</t>
+  </si>
+  <si>
+    <t>beef</t>
+  </si>
+  <si>
+    <t>manzo</t>
+  </si>
+  <si>
+    <t>chicken</t>
+  </si>
+  <si>
+    <t>pollo</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <t>piede</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>testa</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>mano</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>corpo</t>
+  </si>
+  <si>
+    <t>doctor</t>
+  </si>
+  <si>
+    <t>dottore</t>
+  </si>
+  <si>
+    <t>salesman</t>
+  </si>
+  <si>
+    <t>venditore</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -273,6 +384,15 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Saturday, 18 Mar 19:57</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Saturday, 18 Mar 20:11</t>
   </si>
 </sst>
 </file>
@@ -280,23 +400,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <color rgb="FF252525"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <color rgb="FF000000"/>
-      <sz val="14"/>
     </font>
   </fonts>
   <fills count="3">
@@ -325,10 +435,8 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -605,10 +713,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -618,331 +726,483 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>42</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>50</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>52</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>54</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>56</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>58</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>60</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>62</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>64</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>66</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>68</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>70</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>72</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>74</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>76</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>78</v>
       </c>
     </row>
     <row customHeight="1" ht="18" r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -956,10 +1216,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="A2:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -969,24 +1229,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>83</v>
+      <c r="A1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>